<commit_message>
[Nico] - Writing v1.5 - Updated Figure 5
</commit_message>
<xml_diff>
--- a/excels/classif2.xlsx
+++ b/excels/classif2.xlsx
@@ -1105,24 +1105,26 @@
   </sheetPr>
   <dimension ref="A1:P86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F94" activeCellId="0" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,7 +2412,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.14"/>

</xml_diff>